<commit_message>
toilet estimate change of indrayani mandir
</commit_message>
<xml_diff>
--- a/ofc/estimates/toilet (भैपरी आउने बिबिध पुँजिगत खर्च).xlsx
+++ b/ofc/estimates/toilet (भैपरी आउने बिबिध पुँजिगत खर्च).xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="estimated upabhokta" sheetId="12" r:id="rId1"/>
@@ -33,13 +33,13 @@
     <definedName name="description_783">[2]Abstract!$B$301</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">'estimated quotation'!$A$1:$K$58</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'estimated upabhokta'!$A$1:$K$67</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">quotation!$A$1:$K$57</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">quotation!$A$1:$K$63</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="3">'estimated quotation'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'estimated upabhokta'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">quotation!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="94">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -377,14 +377,32 @@
   <si>
     <t>Grand total</t>
   </si>
+  <si>
+    <t>F.Y.: 2081/82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date:              </t>
+  </si>
+  <si>
+    <t>Detail Estimated Sheet</t>
+  </si>
+  <si>
+    <t>UPVC Casement Window(frame 60*60 mm, sash 60*78mm White Colour With 5mm Glass)</t>
+  </si>
+  <si>
+    <t>-Window</t>
+  </si>
+  <si>
+    <t>UPVC Singl Door with full pannel (frame 60*60mm sash 60X100mm) white colour with panel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -591,9 +609,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -601,7 +619,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,7 +641,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -639,7 +657,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -648,7 +666,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -657,7 +675,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -676,7 +694,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -711,7 +729,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -735,9 +753,25 @@
     <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -750,21 +784,20 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -787,29 +820,17 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1231,101 +1252,101 @@
       <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
@@ -1335,31 +1356,31 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -1394,7 +1415,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>1</v>
       </c>
@@ -1418,7 +1439,7 @@
       <c r="R9" s="31"/>
       <c r="S9" s="31"/>
     </row>
-    <row r="10" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="37" t="s">
         <v>46</v>
@@ -1455,7 +1476,7 @@
       <c r="R10" s="31"/>
       <c r="S10" s="31"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="37" t="s">
         <v>47</v>
@@ -1489,7 +1510,7 @@
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="37" t="s">
         <v>48</v>
@@ -1523,7 +1544,7 @@
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="37" t="s">
         <v>49</v>
@@ -1557,7 +1578,7 @@
       <c r="R13" s="31"/>
       <c r="S13" s="31"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="37" t="s">
         <v>50</v>
@@ -1591,7 +1612,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="37" t="s">
         <v>56</v>
@@ -1625,7 +1646,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="31"/>
     </row>
-    <row r="16" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="37" t="s">
         <v>60</v>
@@ -1662,7 +1683,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="31"/>
     </row>
-    <row r="17" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="37" t="s">
         <v>61</v>
@@ -1699,7 +1720,7 @@
       <c r="R17" s="31"/>
       <c r="S17" s="31"/>
     </row>
-    <row r="18" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="37" t="s">
         <v>62</v>
@@ -1736,7 +1757,7 @@
       <c r="R18" s="31"/>
       <c r="S18" s="31"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="37" t="s">
         <v>85</v>
@@ -1770,7 +1791,7 @@
       <c r="R19" s="31"/>
       <c r="S19" s="31"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="37" t="s">
         <v>64</v>
@@ -1804,7 +1825,7 @@
       <c r="R20" s="31"/>
       <c r="S20" s="31"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="37" t="s">
         <v>51</v>
@@ -1841,7 +1862,7 @@
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="37" t="s">
         <v>54</v>
@@ -1878,7 +1899,7 @@
       <c r="R22" s="31"/>
       <c r="S22" s="31"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="37" t="s">
         <v>55</v>
@@ -1912,7 +1933,7 @@
       <c r="R23" s="31"/>
       <c r="S23" s="31"/>
     </row>
-    <row r="24" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="37" t="s">
         <v>57</v>
@@ -1946,7 +1967,7 @@
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="37" t="s">
         <v>59</v>
@@ -1980,7 +2001,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="37" t="s">
         <v>65</v>
@@ -2014,7 +2035,7 @@
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="37" t="s">
         <v>66</v>
@@ -2048,7 +2069,7 @@
       <c r="R27" s="31"/>
       <c r="S27" s="31"/>
     </row>
-    <row r="28" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="37" t="s">
         <v>67</v>
@@ -2082,7 +2103,7 @@
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="46" t="s">
         <v>40</v>
@@ -2100,7 +2121,7 @@
       </c>
       <c r="K29" s="16"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="46"/>
       <c r="C30" s="47"/>
@@ -2113,7 +2134,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="44">
         <v>2</v>
       </c>
@@ -2130,7 +2151,7 @@
       <c r="J31" s="41"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
       <c r="B32" s="46" t="s">
         <v>73</v>
@@ -2156,7 +2177,7 @@
       <c r="J32" s="45"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
       <c r="B33" s="46" t="s">
         <v>74</v>
@@ -2182,7 +2203,7 @@
       <c r="J33" s="45"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="46" t="s">
         <v>75</v>
@@ -2209,7 +2230,7 @@
       <c r="J34" s="45"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="46" t="s">
         <v>76</v>
@@ -2234,7 +2255,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" s="46" t="s">
         <v>39</v>
@@ -2259,7 +2280,7 @@
       </c>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44"/>
       <c r="B37" s="46" t="s">
         <v>40</v>
@@ -2277,7 +2298,7 @@
       </c>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="44"/>
       <c r="B38" s="46"/>
       <c r="C38" s="47"/>
@@ -2290,7 +2311,7 @@
       <c r="J38" s="41"/>
       <c r="K38" s="16"/>
     </row>
-    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="44">
         <v>3</v>
       </c>
@@ -2307,7 +2328,7 @@
       <c r="J39" s="41"/>
       <c r="K39" s="16"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="44"/>
       <c r="B40" s="46" t="s">
         <v>81</v>
@@ -2327,7 +2348,7 @@
       <c r="J40" s="9"/>
       <c r="K40" s="16"/>
     </row>
-    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="44"/>
       <c r="B41" s="46" t="s">
         <v>39</v>
@@ -2352,7 +2373,7 @@
       </c>
       <c r="K41" s="16"/>
     </row>
-    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44"/>
       <c r="B42" s="46" t="s">
         <v>40</v>
@@ -2370,7 +2391,7 @@
       </c>
       <c r="K42" s="16"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="44"/>
       <c r="B43" s="46"/>
       <c r="C43" s="47"/>
@@ -2383,7 +2404,7 @@
       <c r="J43" s="41"/>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="1:11" ht="65.400000000000006" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="66.75" x14ac:dyDescent="0.25">
       <c r="A44" s="44">
         <v>4</v>
       </c>
@@ -2400,7 +2421,7 @@
       <c r="J44" s="41"/>
       <c r="K44" s="16"/>
     </row>
-    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44"/>
       <c r="B45" s="46" t="s">
         <v>74</v>
@@ -2426,7 +2447,7 @@
       <c r="J45" s="45"/>
       <c r="K45" s="16"/>
     </row>
-    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44"/>
       <c r="B46" s="46" t="s">
         <v>78</v>
@@ -2452,7 +2473,7 @@
       <c r="J46" s="45"/>
       <c r="K46" s="16"/>
     </row>
-    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44"/>
       <c r="B47" s="46" t="s">
         <v>75</v>
@@ -2479,7 +2500,7 @@
       <c r="J47" s="45"/>
       <c r="K47" s="16"/>
     </row>
-    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
       <c r="B48" s="46" t="s">
         <v>39</v>
@@ -2504,7 +2525,7 @@
       </c>
       <c r="K48" s="16"/>
     </row>
-    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
       <c r="B49" s="46" t="s">
         <v>40</v>
@@ -2522,7 +2543,7 @@
       </c>
       <c r="K49" s="16"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="26"/>
       <c r="B50" s="30"/>
       <c r="C50" s="27"/>
@@ -2542,7 +2563,7 @@
       <c r="R50" s="31"/>
       <c r="S50" s="31"/>
     </row>
-    <row r="51" spans="1:20" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A51" s="26">
         <v>5</v>
       </c>
@@ -2566,7 +2587,7 @@
       <c r="R51" s="31"/>
       <c r="S51" s="31"/>
     </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="44"/>
       <c r="B52" s="46" t="s">
         <v>84</v>
@@ -2592,7 +2613,7 @@
       <c r="J52" s="45"/>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="44"/>
       <c r="B53" s="46" t="s">
         <v>39</v>
@@ -2617,7 +2638,7 @@
       </c>
       <c r="K53" s="16"/>
     </row>
-    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
       <c r="B54" s="46" t="s">
         <v>40</v>
@@ -2635,7 +2656,7 @@
       </c>
       <c r="K54" s="16"/>
     </row>
-    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="44"/>
       <c r="B55" s="46"/>
       <c r="C55" s="47"/>
@@ -2648,7 +2669,7 @@
       <c r="J55" s="41"/>
       <c r="K55" s="16"/>
     </row>
-    <row r="56" spans="1:20" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="26">
         <v>6</v>
       </c>
@@ -2684,7 +2705,7 @@
       <c r="R56" s="31"/>
       <c r="S56" s="31"/>
     </row>
-    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="44"/>
       <c r="B57" s="46"/>
       <c r="C57" s="47"/>
@@ -2697,7 +2718,7 @@
       <c r="J57" s="45"/>
       <c r="K57" s="16"/>
     </row>
-    <row r="58" spans="1:20" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A58" s="26">
         <v>7</v>
       </c>
@@ -2734,7 +2755,7 @@
       <c r="S58" s="18"/>
       <c r="T58" s="18"/>
     </row>
-    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="26"/>
       <c r="B59" s="30"/>
       <c r="C59" s="27"/>
@@ -2755,7 +2776,7 @@
       <c r="S59" s="18"/>
       <c r="T59" s="18"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="44"/>
       <c r="B60" s="51" t="s">
         <v>16</v>
@@ -2773,15 +2794,15 @@
       </c>
       <c r="K60" s="16"/>
     </row>
-    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B62" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C62" s="60">
+      <c r="C62" s="55">
         <f>J60</f>
         <v>191191.43300038262</v>
       </c>
-      <c r="D62" s="61"/>
+      <c r="D62" s="56"/>
       <c r="E62" s="14">
         <v>100</v>
       </c>
@@ -2792,72 +2813,78 @@
       <c r="J62" s="21"/>
       <c r="K62" s="22"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B63" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="C63" s="63">
+      <c r="C63" s="59">
         <v>160000</v>
       </c>
-      <c r="D63" s="64"/>
+      <c r="D63" s="60"/>
       <c r="E63" s="14"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B64" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="63">
+      <c r="C64" s="59">
         <f>C63-C66-C67</f>
         <v>152000</v>
       </c>
-      <c r="D64" s="64"/>
+      <c r="D64" s="60"/>
       <c r="E64" s="14">
         <f>C64/C62*100</f>
         <v>79.50147013108888</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B65" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C65" s="65">
+      <c r="C65" s="61">
         <f>C62-C64</f>
         <v>39191.433000382618</v>
       </c>
-      <c r="D65" s="65"/>
+      <c r="D65" s="61"/>
       <c r="E65" s="14">
         <f>100-E64</f>
         <v>20.49852986891112</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C66" s="60">
+      <c r="C66" s="55">
         <f>C63*0.03</f>
         <v>4800</v>
       </c>
-      <c r="D66" s="61"/>
+      <c r="D66" s="56"/>
       <c r="E66" s="14">
         <v>3</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B67" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C67" s="60">
+      <c r="C67" s="55">
         <f>C63*0.02</f>
         <v>3200</v>
       </c>
-      <c r="D67" s="61"/>
+      <c r="D67" s="56"/>
       <c r="E67" s="14">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
     <mergeCell ref="A7:F7"/>
@@ -2866,12 +2893,6 @@
     <mergeCell ref="C63:D63"/>
     <mergeCell ref="C64:D64"/>
     <mergeCell ref="C65:D65"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2893,107 +2914,107 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
-    <col min="13" max="13" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="75" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="68" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="I1" s="75"/>
-      <c r="J1" s="75"/>
-      <c r="K1" s="75"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="76" t="s">
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="69" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="76"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="69"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="77" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="70" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="77"/>
-      <c r="C5" s="77"/>
-      <c r="D5" s="77"/>
-      <c r="E5" s="77"/>
-      <c r="F5" s="77"/>
-      <c r="G5" s="77"/>
-      <c r="H5" s="77"/>
-      <c r="I5" s="77"/>
-      <c r="J5" s="77"/>
-      <c r="K5" s="77"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>18</v>
       </c>
       <c r="B6" s="10"/>
-      <c r="C6" s="73" t="e">
+      <c r="C6" s="66" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="74"/>
+      <c r="D6" s="67"/>
       <c r="E6" s="11"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
@@ -3001,13 +3022,13 @@
         <v>19</v>
       </c>
       <c r="I6" s="10"/>
-      <c r="J6" s="73" t="e">
+      <c r="J6" s="66" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="74"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="67"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>28</v>
       </c>
@@ -3016,75 +3037,75 @@
       <c r="D7" s="12"/>
       <c r="F7" s="38"/>
       <c r="G7" s="38"/>
-      <c r="I7" s="69" t="s">
+      <c r="I7" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="J7" s="69"/>
-      <c r="K7" s="69"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="68" t="str">
+      <c r="J7" s="74"/>
+      <c r="K7" s="74"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="73" t="str">
         <f>'estimated upabhokta'!A6</f>
         <v>Project:- इन्द्रायणी सार्वजनिक शौचालय बनाउने काम  (भैपरी आउने बिबिध पुँजिगत खर्च)</v>
       </c>
-      <c r="B8" s="68"/>
-      <c r="C8" s="68"/>
-      <c r="D8" s="68"/>
-      <c r="E8" s="68"/>
-      <c r="F8" s="68"/>
-      <c r="I8" s="70" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="I8" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="71" t="str">
+      <c r="J8" s="75"/>
+      <c r="K8" s="75"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="76" t="str">
         <f>'estimated upabhokta'!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="71"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="I9" s="70" t="s">
+      <c r="B9" s="76"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="I9" s="75" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="66" t="s">
+      <c r="J9" s="75"/>
+      <c r="K9" s="75"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="66" t="s">
+      <c r="B11" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="66" t="s">
+      <c r="C11" s="71" t="s">
         <v>11</v>
       </c>
-      <c r="D11" s="72" t="s">
+      <c r="D11" s="77" t="s">
         <v>22</v>
       </c>
-      <c r="E11" s="72"/>
-      <c r="F11" s="72"/>
-      <c r="G11" s="72" t="s">
+      <c r="E11" s="77"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="72"/>
-      <c r="I11" s="72"/>
-      <c r="J11" s="66" t="s">
+      <c r="H11" s="77"/>
+      <c r="I11" s="77"/>
+      <c r="J11" s="71" t="s">
         <v>24</v>
       </c>
-      <c r="K11" s="67" t="s">
+      <c r="K11" s="72" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="66"/>
-      <c r="B12" s="66"/>
-      <c r="C12" s="66"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="71"/>
+      <c r="B12" s="71"/>
+      <c r="C12" s="71"/>
       <c r="D12" s="13" t="s">
         <v>25</v>
       </c>
@@ -3103,10 +3124,10 @@
       <c r="I12" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="66"/>
-      <c r="K12" s="67"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="J12" s="71"/>
+      <c r="K12" s="72"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="33">
         <f>'estimated upabhokta'!A9</f>
         <v>1</v>
@@ -3149,7 +3170,7 @@
       </c>
       <c r="K13" s="17"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="33"/>
       <c r="B14" s="36" t="str">
         <f>'estimated upabhokta'!B29</f>
@@ -3174,7 +3195,7 @@
       </c>
       <c r="K14" s="17"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="33"/>
       <c r="B15" s="36"/>
       <c r="C15" s="14"/>
@@ -3187,7 +3208,7 @@
       <c r="J15" s="34"/>
       <c r="K15" s="17"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="33">
         <f>'estimated upabhokta'!A58</f>
         <v>7</v>
@@ -3230,7 +3251,7 @@
       </c>
       <c r="K16" s="17"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="35"/>
       <c r="B17" s="35"/>
       <c r="C17" s="14"/>
@@ -3243,7 +3264,7 @@
       <c r="J17" s="34"/>
       <c r="K17" s="17"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>15</v>
@@ -3269,13 +3290,6 @@
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3288,6 +3302,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3303,107 +3324,107 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T59"/>
+  <dimension ref="A1:T63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="I63" sqref="I63"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="65" t="s">
+        <v>90</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>82</v>
       </c>
@@ -3413,31 +3434,31 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="H6" s="58" t="s">
+        <v>88</v>
+      </c>
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -3472,7 +3493,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>1</v>
       </c>
@@ -3496,7 +3517,7 @@
       <c r="R9" s="31"/>
       <c r="S9" s="31"/>
     </row>
-    <row r="10" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="37" t="s">
         <v>46</v>
@@ -3533,7 +3554,7 @@
       <c r="R10" s="31"/>
       <c r="S10" s="31"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="37" t="s">
         <v>47</v>
@@ -3567,7 +3588,7 @@
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="37" t="s">
         <v>48</v>
@@ -3601,7 +3622,7 @@
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="37" t="s">
         <v>49</v>
@@ -3635,7 +3656,7 @@
       <c r="R13" s="31"/>
       <c r="S13" s="31"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="37" t="s">
         <v>50</v>
@@ -3669,7 +3690,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="37" t="s">
         <v>56</v>
@@ -3703,7 +3724,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="31"/>
     </row>
-    <row r="16" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="37" t="s">
         <v>60</v>
@@ -3740,7 +3761,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="31"/>
     </row>
-    <row r="17" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="37" t="s">
         <v>61</v>
@@ -3777,7 +3798,7 @@
       <c r="R17" s="31"/>
       <c r="S17" s="31"/>
     </row>
-    <row r="18" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="37" t="s">
         <v>62</v>
@@ -3814,7 +3835,7 @@
       <c r="R18" s="31"/>
       <c r="S18" s="31"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="37" t="s">
         <v>85</v>
@@ -3848,7 +3869,7 @@
       <c r="R19" s="31"/>
       <c r="S19" s="31"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="37" t="s">
         <v>64</v>
@@ -3882,7 +3903,7 @@
       <c r="R20" s="31"/>
       <c r="S20" s="31"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="37" t="s">
         <v>51</v>
@@ -3919,7 +3940,7 @@
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="37" t="s">
         <v>54</v>
@@ -3956,7 +3977,7 @@
       <c r="R22" s="31"/>
       <c r="S22" s="31"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="37" t="s">
         <v>55</v>
@@ -3990,7 +4011,7 @@
       <c r="R23" s="31"/>
       <c r="S23" s="31"/>
     </row>
-    <row r="24" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="37" t="s">
         <v>57</v>
@@ -4024,7 +4045,7 @@
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="37" t="s">
         <v>59</v>
@@ -4058,7 +4079,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="37" t="s">
         <v>65</v>
@@ -4092,7 +4113,7 @@
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="37" t="s">
         <v>66</v>
@@ -4126,7 +4147,7 @@
       <c r="R27" s="31"/>
       <c r="S27" s="31"/>
     </row>
-    <row r="28" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="37" t="s">
         <v>67</v>
@@ -4160,7 +4181,7 @@
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="44"/>
       <c r="B29" s="46"/>
       <c r="C29" s="47"/>
@@ -4173,7 +4194,7 @@
       <c r="J29" s="41"/>
       <c r="K29" s="16"/>
     </row>
-    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="44">
         <v>2</v>
       </c>
@@ -4190,7 +4211,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="44"/>
       <c r="B31" s="46" t="s">
         <v>73</v>
@@ -4216,7 +4237,7 @@
       <c r="J31" s="45"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
       <c r="B32" s="46" t="s">
         <v>74</v>
@@ -4242,7 +4263,7 @@
       <c r="J32" s="45"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
       <c r="B33" s="46" t="s">
         <v>75</v>
@@ -4269,7 +4290,7 @@
       <c r="J33" s="45"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="46" t="s">
         <v>76</v>
@@ -4294,7 +4315,7 @@
       <c r="J34" s="45"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="46" t="s">
         <v>39</v>
@@ -4320,7 +4341,7 @@
       </c>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" s="46"/>
       <c r="C36" s="47"/>
@@ -4333,7 +4354,7 @@
       <c r="J36" s="41"/>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="44">
         <v>3</v>
       </c>
@@ -4350,7 +4371,7 @@
       <c r="J37" s="41"/>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38" s="44"/>
       <c r="B38" s="46" t="s">
         <v>81</v>
@@ -4370,7 +4391,7 @@
       <c r="J38" s="9"/>
       <c r="K38" s="16"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="44"/>
       <c r="B39" s="46" t="s">
         <v>39</v>
@@ -4396,7 +4417,7 @@
       </c>
       <c r="K39" s="16"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="44"/>
       <c r="B40" s="46"/>
       <c r="C40" s="47"/>
@@ -4409,7 +4430,7 @@
       <c r="J40" s="41"/>
       <c r="K40" s="16"/>
     </row>
-    <row r="41" spans="1:19" ht="65.400000000000006" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="79.5" x14ac:dyDescent="0.25">
       <c r="A41" s="44">
         <v>4</v>
       </c>
@@ -4426,7 +4447,7 @@
       <c r="J41" s="41"/>
       <c r="K41" s="16"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="44"/>
       <c r="B42" s="46" t="s">
         <v>74</v>
@@ -4452,7 +4473,7 @@
       <c r="J42" s="45"/>
       <c r="K42" s="16"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44"/>
       <c r="B43" s="46" t="s">
         <v>78</v>
@@ -4478,7 +4499,7 @@
       <c r="J43" s="45"/>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44"/>
       <c r="B44" s="46" t="s">
         <v>75</v>
@@ -4505,7 +4526,7 @@
       <c r="J44" s="45"/>
       <c r="K44" s="16"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44"/>
       <c r="B45" s="46" t="s">
         <v>39</v>
@@ -4531,7 +4552,7 @@
       </c>
       <c r="K45" s="16"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
       <c r="B46" s="30"/>
       <c r="C46" s="27"/>
@@ -4551,12 +4572,12 @@
       <c r="R46" s="31"/>
       <c r="S46" s="31"/>
     </row>
-    <row r="47" spans="1:19" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A47" s="26">
         <v>5</v>
       </c>
       <c r="B47" s="54" t="s">
-        <v>83</v>
+        <v>93</v>
       </c>
       <c r="C47" s="54"/>
       <c r="D47" s="28"/>
@@ -4575,7 +4596,7 @@
       <c r="R47" s="31"/>
       <c r="S47" s="31"/>
     </row>
-    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="44"/>
       <c r="B48" s="46" t="s">
         <v>84</v>
@@ -4601,7 +4622,7 @@
       <c r="J48" s="45"/>
       <c r="K48" s="16"/>
     </row>
-    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
       <c r="B49" s="46" t="s">
         <v>39</v>
@@ -4618,215 +4639,295 @@
         <v>71</v>
       </c>
       <c r="I49" s="45">
-        <f>1.15*7069.31</f>
-        <v>8129.7065000000002</v>
+        <v>10055.6</v>
       </c>
       <c r="J49" s="45">
         <f>G49*I49</f>
-        <v>31220.451661078936</v>
+        <v>38616.446205425171</v>
       </c>
       <c r="K49" s="16"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44"/>
       <c r="B50" s="46"/>
       <c r="C50" s="47"/>
       <c r="D50" s="14"/>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="48"/>
-      <c r="H50" s="48"/>
-      <c r="I50" s="48"/>
-      <c r="J50" s="41"/>
+      <c r="G50" s="45"/>
+      <c r="H50" s="45"/>
+      <c r="I50" s="45"/>
+      <c r="J50" s="45"/>
       <c r="K50" s="16"/>
     </row>
-    <row r="51" spans="1:20" ht="41.4" x14ac:dyDescent="0.3">
-      <c r="A51" s="26">
+    <row r="51" spans="1:20" ht="38.25" x14ac:dyDescent="0.25">
+      <c r="A51" s="44">
         <v>6</v>
       </c>
-      <c r="B51" s="53" t="s">
-        <v>86</v>
-      </c>
-      <c r="C51" s="27">
-        <v>1</v>
-      </c>
-      <c r="D51" s="28"/>
-      <c r="E51" s="28"/>
-      <c r="F51" s="29"/>
-      <c r="G51" s="14">
-        <f>PRODUCT(C51:F51)</f>
-        <v>1</v>
-      </c>
-      <c r="H51" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="I51" s="40">
-        <v>20000</v>
-      </c>
-      <c r="J51" s="41">
-        <f>G51*I51</f>
-        <v>20000</v>
-      </c>
-      <c r="K51" s="29"/>
-      <c r="M51" s="31"/>
-      <c r="N51" s="1"/>
-      <c r="O51" s="1"/>
-      <c r="P51" s="1"/>
-      <c r="Q51" s="1"/>
-      <c r="R51" s="31"/>
-      <c r="S51" s="31"/>
-    </row>
-    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B51" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="C51" s="54"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+      <c r="J51" s="41"/>
+      <c r="K51" s="16"/>
+    </row>
+    <row r="52" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="44"/>
-      <c r="B52" s="46"/>
-      <c r="C52" s="47"/>
+      <c r="B52" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="C52" s="47">
+        <v>2</v>
+      </c>
       <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="14"/>
-      <c r="G52" s="45"/>
-      <c r="H52" s="45"/>
+      <c r="E52" s="14">
+        <f>E34</f>
+        <v>1.2</v>
+      </c>
+      <c r="F52" s="14">
+        <f>F34</f>
+        <v>0.75</v>
+      </c>
+      <c r="G52" s="14">
+        <f t="shared" ref="G52" si="5">PRODUCT(C52:F52)</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="H52" s="48"/>
       <c r="I52" s="45"/>
       <c r="J52" s="45"/>
       <c r="K52" s="16"/>
     </row>
-    <row r="53" spans="1:20" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A53" s="26">
-        <v>7</v>
-      </c>
-      <c r="B53" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="C53" s="27">
-        <v>1</v>
-      </c>
-      <c r="D53" s="28"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
+    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="44"/>
+      <c r="B53" s="46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C53" s="47"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
       <c r="G53" s="45">
-        <f t="shared" ref="G53" si="5">PRODUCT(C53:F53)</f>
-        <v>1</v>
-      </c>
-      <c r="H53" s="39" t="s">
-        <v>30</v>
-      </c>
-      <c r="I53" s="40">
-        <v>500</v>
+        <f>SUM(G52)</f>
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="H53" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="I53" s="45">
+        <v>9047.0499999999993</v>
       </c>
       <c r="J53" s="45">
         <f>G53*I53</f>
+        <v>16284.689999999997</v>
+      </c>
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="44"/>
+      <c r="B54" s="81"/>
+      <c r="C54" s="81"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="48"/>
+      <c r="I54" s="48"/>
+      <c r="J54" s="41"/>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="26">
+        <v>7</v>
+      </c>
+      <c r="B55" s="53" t="s">
+        <v>86</v>
+      </c>
+      <c r="C55" s="27">
+        <v>1</v>
+      </c>
+      <c r="D55" s="28"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="29"/>
+      <c r="G55" s="14">
+        <f>PRODUCT(C55:F55)</f>
+        <v>1</v>
+      </c>
+      <c r="H55" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="I55" s="40">
+        <v>20000</v>
+      </c>
+      <c r="J55" s="41">
+        <f>G55*I55</f>
+        <v>20000</v>
+      </c>
+      <c r="K55" s="29"/>
+      <c r="M55" s="31"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="31"/>
+      <c r="S55" s="31"/>
+    </row>
+    <row r="56" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="44"/>
+      <c r="B56" s="46"/>
+      <c r="C56" s="47"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="45"/>
+      <c r="H56" s="45"/>
+      <c r="I56" s="45"/>
+      <c r="J56" s="45"/>
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="1:20" ht="19.5" x14ac:dyDescent="0.25">
+      <c r="A57" s="26">
+        <v>8</v>
+      </c>
+      <c r="B57" s="42" t="s">
+        <v>29</v>
+      </c>
+      <c r="C57" s="27">
+        <v>1</v>
+      </c>
+      <c r="D57" s="28"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="29"/>
+      <c r="G57" s="45">
+        <f t="shared" ref="G57" si="6">PRODUCT(C57:F57)</f>
+        <v>1</v>
+      </c>
+      <c r="H57" s="39" t="s">
+        <v>30</v>
+      </c>
+      <c r="I57" s="40">
         <v>500</v>
       </c>
-      <c r="K53" s="29"/>
-      <c r="M53" s="31"/>
-      <c r="N53" s="18"/>
-      <c r="O53" s="18"/>
-      <c r="P53" s="18"/>
-      <c r="Q53" s="18"/>
-      <c r="R53" s="18"/>
-      <c r="S53" s="18"/>
-      <c r="T53" s="18"/>
-    </row>
-    <row r="54" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="26"/>
-      <c r="B54" s="30"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="29"/>
-      <c r="F54" s="29"/>
-      <c r="G54" s="40"/>
-      <c r="H54" s="39"/>
-      <c r="I54" s="40"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="29"/>
-      <c r="M54" s="31"/>
-      <c r="N54" s="18"/>
-      <c r="O54" s="18"/>
-      <c r="P54" s="18"/>
-      <c r="Q54" s="18"/>
-      <c r="R54" s="18"/>
-      <c r="S54" s="18"/>
-      <c r="T54" s="18"/>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A55" s="44"/>
-      <c r="B55" s="51" t="s">
+      <c r="J57" s="45">
+        <f>G57*I57</f>
+        <v>500</v>
+      </c>
+      <c r="K57" s="29"/>
+      <c r="M57" s="31"/>
+      <c r="N57" s="18"/>
+      <c r="O57" s="18"/>
+      <c r="P57" s="18"/>
+      <c r="Q57" s="18"/>
+      <c r="R57" s="18"/>
+      <c r="S57" s="18"/>
+      <c r="T57" s="18"/>
+    </row>
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="26"/>
+      <c r="B58" s="30"/>
+      <c r="C58" s="27"/>
+      <c r="D58" s="28"/>
+      <c r="E58" s="29"/>
+      <c r="F58" s="29"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="39"/>
+      <c r="I58" s="40"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="29"/>
+      <c r="M58" s="31"/>
+      <c r="N58" s="18"/>
+      <c r="O58" s="18"/>
+      <c r="P58" s="18"/>
+      <c r="Q58" s="18"/>
+      <c r="R58" s="18"/>
+      <c r="S58" s="18"/>
+      <c r="T58" s="18"/>
+    </row>
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A59" s="44"/>
+      <c r="B59" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C55" s="47"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="14"/>
-      <c r="G55" s="45"/>
-      <c r="H55" s="45"/>
-      <c r="I55" s="45"/>
-      <c r="J55" s="45">
-        <f>SUM(J9:J53)</f>
-        <v>200345.3818182718</v>
-      </c>
-      <c r="K55" s="16"/>
-    </row>
-    <row r="57" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B57" s="44" t="s">
+      <c r="C59" s="47"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="45"/>
+      <c r="H59" s="45"/>
+      <c r="I59" s="45"/>
+      <c r="J59" s="45">
+        <f>SUM(J9:J57)</f>
+        <v>224026.06636261803</v>
+      </c>
+      <c r="K59" s="16"/>
+    </row>
+    <row r="61" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="44" t="s">
         <v>26</v>
       </c>
-      <c r="C57" s="79">
-        <f>J55</f>
-        <v>200345.3818182718</v>
-      </c>
-      <c r="D57" s="79"/>
-      <c r="E57" s="18"/>
-      <c r="F57" s="19"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="20"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="22"/>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B58" s="9" t="s">
+      <c r="C61" s="79">
+        <f>J59</f>
+        <v>224026.06636261803</v>
+      </c>
+      <c r="D61" s="79"/>
+      <c r="E61" s="18"/>
+      <c r="F61" s="19"/>
+      <c r="G61" s="18"/>
+      <c r="H61" s="20"/>
+      <c r="I61" s="21"/>
+      <c r="J61" s="22"/>
+    </row>
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B62" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="C58" s="80">
-        <f>13%*C57</f>
-        <v>26044.899636375336</v>
-      </c>
-      <c r="D58" s="80"/>
-      <c r="F58" s="7"/>
-      <c r="J58"/>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="B59" s="9" t="s">
+      <c r="C62" s="78">
+        <f>13%*C61</f>
+        <v>29123.388627140346</v>
+      </c>
+      <c r="D62" s="78"/>
+      <c r="F62" s="7"/>
+      <c r="J62"/>
+    </row>
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="B63" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="C59" s="80">
-        <f>SUM(C57:D58)</f>
-        <v>226390.28145464713</v>
-      </c>
-      <c r="D59" s="80"/>
-      <c r="F59" s="7"/>
-      <c r="J59"/>
+      <c r="C63" s="78">
+        <f>SUM(C61:D62)</f>
+        <v>253149.45498975838</v>
+      </c>
+      <c r="D63" s="78"/>
+      <c r="F63" s="7"/>
+      <c r="J63"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C58:D58"/>
-    <mergeCell ref="C59:D59"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="C62:D62"/>
+    <mergeCell ref="C63:D63"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C61:D61"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:        
-Er. Milan Phuyal&amp;RApproved By:                 
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter xml:space="preserve">&amp;LPrepared By:
+&amp;CChecked By:        
+&amp;RApproved By:                 
+</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -4839,101 +4940,101 @@
       <selection activeCell="E50" sqref="E50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" style="7" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" customWidth="1"/>
-    <col min="5" max="5" width="7.88671875" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" customWidth="1"/>
-    <col min="7" max="7" width="8.5546875" style="7" customWidth="1"/>
-    <col min="8" max="8" width="5.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" style="7" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.33203125" customWidth="1"/>
-    <col min="14" max="14" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.85546875" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="7" max="7" width="8.5703125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="5.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" style="7" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.28515625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.109375" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="56" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="62" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="56"/>
-      <c r="C1" s="56"/>
-      <c r="D1" s="56"/>
-      <c r="E1" s="56"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="57" t="s">
+      <c r="B1" s="62"/>
+      <c r="C1" s="62"/>
+      <c r="D1" s="62"/>
+      <c r="E1" s="62"/>
+      <c r="F1" s="62"/>
+      <c r="G1" s="62"/>
+      <c r="H1" s="62"/>
+      <c r="I1" s="62"/>
+      <c r="J1" s="62"/>
+      <c r="K1" s="62"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="57"/>
-      <c r="C2" s="57"/>
-      <c r="D2" s="57"/>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="58" t="s">
+      <c r="B3" s="64"/>
+      <c r="C3" s="64"/>
+      <c r="D3" s="64"/>
+      <c r="E3" s="64"/>
+      <c r="F3" s="64"/>
+      <c r="G3" s="64"/>
+      <c r="H3" s="64"/>
+      <c r="I3" s="64"/>
+      <c r="J3" s="64"/>
+      <c r="K3" s="64"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="64" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="59" t="s">
+      <c r="B4" s="64"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="59"/>
-      <c r="C5" s="59"/>
-      <c r="D5" s="59"/>
-      <c r="E5" s="59"/>
-      <c r="F5" s="59"/>
-      <c r="G5" s="59"/>
-      <c r="H5" s="59"/>
-      <c r="I5" s="59"/>
-      <c r="J5" s="59"/>
-      <c r="K5" s="59"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B5" s="65"/>
+      <c r="C5" s="65"/>
+      <c r="D5" s="65"/>
+      <c r="E5" s="65"/>
+      <c r="F5" s="65"/>
+      <c r="G5" s="65"/>
+      <c r="H5" s="65"/>
+      <c r="I5" s="65"/>
+      <c r="J5" s="65"/>
+      <c r="K5" s="65"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="43" t="s">
         <v>44</v>
       </c>
@@ -4943,31 +5044,31 @@
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="55" t="s">
+      <c r="H6" s="58" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="I6" s="58"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="58"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="57" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="62"/>
-      <c r="C7" s="62"/>
-      <c r="D7" s="62"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="62"/>
+      <c r="B7" s="57"/>
+      <c r="C7" s="57"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="57"/>
+      <c r="F7" s="57"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="58" t="s">
         <v>43</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="58"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="58"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>4</v>
       </c>
@@ -5002,7 +5103,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="26">
         <v>1</v>
       </c>
@@ -5026,7 +5127,7 @@
       <c r="R9" s="31"/>
       <c r="S9" s="31"/>
     </row>
-    <row r="10" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="26"/>
       <c r="B10" s="37" t="s">
         <v>46</v>
@@ -5063,7 +5164,7 @@
       <c r="R10" s="31"/>
       <c r="S10" s="31"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="26"/>
       <c r="B11" s="37" t="s">
         <v>47</v>
@@ -5097,7 +5198,7 @@
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="26"/>
       <c r="B12" s="37" t="s">
         <v>48</v>
@@ -5131,7 +5232,7 @@
       <c r="R12" s="31"/>
       <c r="S12" s="31"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="26"/>
       <c r="B13" s="37" t="s">
         <v>49</v>
@@ -5165,7 +5266,7 @@
       <c r="R13" s="31"/>
       <c r="S13" s="31"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="26"/>
       <c r="B14" s="37" t="s">
         <v>50</v>
@@ -5199,7 +5300,7 @@
       <c r="R14" s="31"/>
       <c r="S14" s="31"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26"/>
       <c r="B15" s="37" t="s">
         <v>56</v>
@@ -5233,7 +5334,7 @@
       <c r="R15" s="31"/>
       <c r="S15" s="31"/>
     </row>
-    <row r="16" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="26"/>
       <c r="B16" s="37" t="s">
         <v>60</v>
@@ -5270,7 +5371,7 @@
       <c r="R16" s="31"/>
       <c r="S16" s="31"/>
     </row>
-    <row r="17" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="26"/>
       <c r="B17" s="37" t="s">
         <v>61</v>
@@ -5307,7 +5408,7 @@
       <c r="R17" s="31"/>
       <c r="S17" s="31"/>
     </row>
-    <row r="18" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="26"/>
       <c r="B18" s="37" t="s">
         <v>62</v>
@@ -5344,7 +5445,7 @@
       <c r="R18" s="31"/>
       <c r="S18" s="31"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="26"/>
       <c r="B19" s="37" t="s">
         <v>63</v>
@@ -5378,7 +5479,7 @@
       <c r="R19" s="31"/>
       <c r="S19" s="31"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="26"/>
       <c r="B20" s="37" t="s">
         <v>64</v>
@@ -5412,7 +5513,7 @@
       <c r="R20" s="31"/>
       <c r="S20" s="31"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="26"/>
       <c r="B21" s="37" t="s">
         <v>51</v>
@@ -5449,7 +5550,7 @@
       <c r="R21" s="31"/>
       <c r="S21" s="31"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="26"/>
       <c r="B22" s="37" t="s">
         <v>54</v>
@@ -5486,7 +5587,7 @@
       <c r="R22" s="31"/>
       <c r="S22" s="31"/>
     </row>
-    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="26"/>
       <c r="B23" s="37" t="s">
         <v>55</v>
@@ -5520,7 +5621,7 @@
       <c r="R23" s="31"/>
       <c r="S23" s="31"/>
     </row>
-    <row r="24" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="26"/>
       <c r="B24" s="37" t="s">
         <v>57</v>
@@ -5554,7 +5655,7 @@
       <c r="R24" s="31"/>
       <c r="S24" s="31"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26"/>
       <c r="B25" s="37" t="s">
         <v>59</v>
@@ -5588,7 +5689,7 @@
       <c r="R25" s="31"/>
       <c r="S25" s="31"/>
     </row>
-    <row r="26" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="26"/>
       <c r="B26" s="37" t="s">
         <v>65</v>
@@ -5622,7 +5723,7 @@
       <c r="R26" s="31"/>
       <c r="S26" s="31"/>
     </row>
-    <row r="27" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="26"/>
       <c r="B27" s="37" t="s">
         <v>66</v>
@@ -5656,7 +5757,7 @@
       <c r="R27" s="31"/>
       <c r="S27" s="31"/>
     </row>
-    <row r="28" spans="1:19" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="26"/>
       <c r="B28" s="37" t="s">
         <v>67</v>
@@ -5690,7 +5791,7 @@
       <c r="R28" s="31"/>
       <c r="S28" s="31"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26"/>
       <c r="B29" s="53" t="s">
         <v>77</v>
@@ -5724,7 +5825,7 @@
       <c r="R29" s="31"/>
       <c r="S29" s="31"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="44"/>
       <c r="B30" s="46"/>
       <c r="C30" s="47"/>
@@ -5737,7 +5838,7 @@
       <c r="J30" s="41"/>
       <c r="K30" s="16"/>
     </row>
-    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="44">
         <v>2</v>
       </c>
@@ -5754,7 +5855,7 @@
       <c r="J31" s="41"/>
       <c r="K31" s="16"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="44"/>
       <c r="B32" s="46" t="s">
         <v>73</v>
@@ -5780,7 +5881,7 @@
       <c r="J32" s="45"/>
       <c r="K32" s="16"/>
     </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="44"/>
       <c r="B33" s="46" t="s">
         <v>74</v>
@@ -5806,7 +5907,7 @@
       <c r="J33" s="45"/>
       <c r="K33" s="16"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="46" t="s">
         <v>75</v>
@@ -5833,7 +5934,7 @@
       <c r="J34" s="45"/>
       <c r="K34" s="16"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="44"/>
       <c r="B35" s="46" t="s">
         <v>76</v>
@@ -5858,7 +5959,7 @@
       <c r="J35" s="45"/>
       <c r="K35" s="16"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="44"/>
       <c r="B36" s="46" t="s">
         <v>39</v>
@@ -5883,7 +5984,7 @@
       </c>
       <c r="K36" s="16"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="44"/>
       <c r="B37" s="46"/>
       <c r="C37" s="47"/>
@@ -5896,7 +5997,7 @@
       <c r="J37" s="41"/>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:19" ht="30" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="44">
         <v>3</v>
       </c>
@@ -5913,7 +6014,7 @@
       <c r="J38" s="41"/>
       <c r="K38" s="16"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="44"/>
       <c r="B39" s="46" t="s">
         <v>81</v>
@@ -5933,7 +6034,7 @@
       <c r="J39" s="9"/>
       <c r="K39" s="16"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="44"/>
       <c r="B40" s="46" t="s">
         <v>39</v>
@@ -5958,7 +6059,7 @@
       </c>
       <c r="K40" s="16"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="44"/>
       <c r="B41" s="46"/>
       <c r="C41" s="47"/>
@@ -5971,7 +6072,7 @@
       <c r="J41" s="41"/>
       <c r="K41" s="16"/>
     </row>
-    <row r="42" spans="1:19" ht="65.400000000000006" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="66.75" x14ac:dyDescent="0.25">
       <c r="A42" s="44">
         <v>4</v>
       </c>
@@ -5988,7 +6089,7 @@
       <c r="J42" s="41"/>
       <c r="K42" s="16"/>
     </row>
-    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44"/>
       <c r="B43" s="46" t="s">
         <v>74</v>
@@ -6014,7 +6115,7 @@
       <c r="J43" s="45"/>
       <c r="K43" s="16"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="44"/>
       <c r="B44" s="46" t="s">
         <v>78</v>
@@ -6040,7 +6141,7 @@
       <c r="J44" s="45"/>
       <c r="K44" s="16"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="44"/>
       <c r="B45" s="46" t="s">
         <v>75</v>
@@ -6067,7 +6168,7 @@
       <c r="J45" s="45"/>
       <c r="K45" s="16"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="44"/>
       <c r="B46" s="46" t="s">
         <v>39</v>
@@ -6092,7 +6193,7 @@
       </c>
       <c r="K46" s="16"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="44"/>
       <c r="B47" s="46"/>
       <c r="C47" s="47"/>
@@ -6105,7 +6206,7 @@
       <c r="J47" s="45"/>
       <c r="K47" s="16"/>
     </row>
-    <row r="48" spans="1:19" ht="105.6" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="114.75" x14ac:dyDescent="0.25">
       <c r="A48" s="26">
         <v>5</v>
       </c>
@@ -6129,7 +6230,7 @@
       <c r="R48" s="31"/>
       <c r="S48" s="31"/>
     </row>
-    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="44"/>
       <c r="B49" s="46" t="s">
         <v>84</v>
@@ -6155,7 +6256,7 @@
       <c r="J49" s="45"/>
       <c r="K49" s="16"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="44"/>
       <c r="B50" s="46" t="s">
         <v>39</v>
@@ -6180,7 +6281,7 @@
       </c>
       <c r="K50" s="16"/>
     </row>
-    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="44"/>
       <c r="B51" s="46"/>
       <c r="C51" s="47"/>
@@ -6193,7 +6294,7 @@
       <c r="J51" s="45"/>
       <c r="K51" s="16"/>
     </row>
-    <row r="52" spans="1:20" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" ht="19.5" x14ac:dyDescent="0.25">
       <c r="A52" s="26">
         <v>6</v>
       </c>
@@ -6230,7 +6331,7 @@
       <c r="S52" s="18"/>
       <c r="T52" s="18"/>
     </row>
-    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="26"/>
       <c r="B53" s="30"/>
       <c r="C53" s="27"/>
@@ -6251,7 +6352,7 @@
       <c r="S53" s="18"/>
       <c r="T53" s="18"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="44"/>
       <c r="B54" s="51" t="s">
         <v>16</v>
@@ -6269,15 +6370,15 @@
       </c>
       <c r="K54" s="16"/>
     </row>
-    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B56" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C56" s="65">
+      <c r="C56" s="61">
         <f>J54</f>
         <v>187772.19644527225</v>
       </c>
-      <c r="D56" s="65"/>
+      <c r="D56" s="61"/>
       <c r="E56" s="19"/>
       <c r="F56" s="18"/>
       <c r="G56" s="19"/>
@@ -6286,41 +6387,41 @@
       <c r="J56" s="21"/>
       <c r="K56" s="22"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B57" s="16" t="s">
         <v>79</v>
       </c>
-      <c r="C57" s="78">
+      <c r="C57" s="80">
         <f>C56*0.13</f>
         <v>24410.385537885391</v>
       </c>
-      <c r="D57" s="78"/>
+      <c r="D57" s="80"/>
       <c r="E57" s="19"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B58" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="C58" s="78">
+      <c r="C58" s="80">
         <f>SUM(C56:D57)</f>
         <v>212182.58198315764</v>
       </c>
-      <c r="D58" s="78"/>
+      <c r="D58" s="80"/>
       <c r="E58" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C56:D56"/>
+    <mergeCell ref="C57:D57"/>
+    <mergeCell ref="C58:D58"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="A2:K2"/>
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C56:D56"/>
-    <mergeCell ref="C57:D57"/>
-    <mergeCell ref="C58:D58"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>